<commit_message>
switch to 1 adsorption column; more oilcane simulations
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_3.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_3.xlsx
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.04773246795729871</v>
+        <v>-0.047730824917233</v>
       </c>
       <c r="D4" t="n">
         <v>0.003529454733178189</v>
@@ -750,10 +750,10 @@
         <v>0.1765836888553475</v>
       </c>
       <c r="I4" t="n">
-        <v>0.04431772209270889</v>
+        <v>0.04431756993270279</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2335887026319771</v>
+        <v>0.2335884120935711</v>
       </c>
       <c r="K4" t="n">
         <v>0.02888201030728041</v>
@@ -786,35 +786,35 @@
         <v>0.01546185229847409</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.002243594873797641</v>
+        <v>-0.002247959897972347</v>
       </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="n">
-        <v>0.01956828193473128</v>
+        <v>0.01957059198282367</v>
       </c>
       <c r="X4" t="n">
-        <v>0.3095123183964927</v>
+        <v>0.3095011949720478</v>
       </c>
       <c r="Y4" t="n">
         <v>0.9980585269303408</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.2351125423645017</v>
+        <v>0.2351140617565624</v>
       </c>
       <c r="AA4" t="n">
-        <v>-0.1016501426260057</v>
+        <v>-0.101643625185745</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.1016501426260057</v>
+        <v>-0.101643625185745</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.1016501426260057</v>
+        <v>-0.101643625185745</v>
       </c>
       <c r="AD4" t="n">
-        <v>-0.1016501426260057</v>
+        <v>-0.101643625185745</v>
       </c>
       <c r="AE4" t="n">
-        <v>-0.1016501426260057</v>
+        <v>-0.101643625185745</v>
       </c>
     </row>
     <row r="5">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0878303429372137</v>
+        <v>0.08783123093724922</v>
       </c>
       <c r="D5" t="n">
         <v>0.007570266830810672</v>
@@ -841,10 +841,10 @@
         <v>0.008470465394818614</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.03709523380380935</v>
+        <v>-0.03709537914781517</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01110641950291556</v>
+        <v>0.01110647796718455</v>
       </c>
       <c r="K5" t="n">
         <v>0.09362077286483089</v>
@@ -877,35 +877,35 @@
         <v>0.1697637390465495</v>
       </c>
       <c r="U5" t="n">
-        <v>0.07684732214773723</v>
+        <v>0.07684672397171328</v>
       </c>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="n">
-        <v>0.002569518534780741</v>
+        <v>0.002569427430777097</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.2757286319891453</v>
+        <v>-0.2757315971412638</v>
       </c>
       <c r="Y5" t="n">
         <v>-0.01175957327038293</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.1731374200454968</v>
+        <v>-0.1731417273736691</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.1996068343842733</v>
+        <v>0.1996081460323258</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.1996068343842733</v>
+        <v>0.1996081460323258</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1996068343842733</v>
+        <v>0.1996081460323258</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.1996068343842733</v>
+        <v>0.1996081460323258</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.1996068343842733</v>
+        <v>0.1996081460323258</v>
       </c>
     </row>
     <row r="6">
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3745722949508917</v>
+        <v>0.3745733247429329</v>
       </c>
       <c r="D6" t="n">
         <v>0.0108233524329341</v>
@@ -932,10 +932,10 @@
         <v>-0.006998576439943056</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.5853825610473024</v>
+        <v>-0.5853824858792993</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1092099056078688</v>
+        <v>0.1092098525704877</v>
       </c>
       <c r="K6" t="n">
         <v>0.01227868311514732</v>
@@ -968,35 +968,35 @@
         <v>0.02901910138476405</v>
       </c>
       <c r="U6" t="n">
-        <v>0.04042368699391764</v>
+        <v>0.04042644526602805</v>
       </c>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="n">
-        <v>-0.02792400063696002</v>
+        <v>-0.02792284402891376</v>
       </c>
       <c r="X6" t="n">
-        <v>0.02006967430678697</v>
+        <v>0.02007452537898101</v>
       </c>
       <c r="Y6" t="n">
         <v>-0.0009923803596952143</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.2385805568072223</v>
+        <v>-0.238582775943311</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.003709672276386891</v>
+        <v>-0.003712417972496718</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.003709672276386891</v>
+        <v>-0.003712417972496718</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.003709672276386891</v>
+        <v>-0.003712417972496718</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.003709672276386891</v>
+        <v>-0.003712417972496718</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.003709672276386891</v>
+        <v>-0.003712417972496718</v>
       </c>
     </row>
     <row r="7">
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.002652137098085483</v>
+        <v>-0.002651539210061568</v>
       </c>
       <c r="D7" t="n">
         <v>-0.004311911308476452</v>
@@ -1023,10 +1023,10 @@
         <v>0.0088485200339408</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.002490883107635324</v>
+        <v>-0.002490862947634518</v>
       </c>
       <c r="J7" t="n">
-        <v>0.01071837620674192</v>
+        <v>0.01071838259099943</v>
       </c>
       <c r="K7" t="n">
         <v>0.006488296195531847</v>
@@ -1059,35 +1059,35 @@
         <v>0.002542265861690634</v>
       </c>
       <c r="U7" t="n">
-        <v>0.003266065330720999</v>
+        <v>0.00326717393876537</v>
       </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="n">
-        <v>0.01725476411419057</v>
+        <v>0.01725452862618114</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.01543777271351091</v>
+        <v>-0.01543446445737858</v>
       </c>
       <c r="Y7" t="n">
         <v>-0.01073480961339238</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.02475407695816308</v>
+        <v>-0.02475265539010621</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.009902626476105058</v>
+        <v>0.009901705164068204</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.009902626476105058</v>
+        <v>0.009901705164068204</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.009902626476105058</v>
+        <v>0.009901705164068204</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.009902626476105058</v>
+        <v>0.009901705164068204</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.009902626476105058</v>
+        <v>0.009901705164068204</v>
       </c>
     </row>
     <row r="8">
@@ -1098,7 +1098,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3516725545469022</v>
+        <v>0.3516726042749041</v>
       </c>
       <c r="D8" t="n">
         <v>0.9999999999999999</v>
@@ -1114,10 +1114,10 @@
         <v>-0.001561537790461512</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7490542425701696</v>
+        <v>0.7490543670821747</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.1485170270381897</v>
+        <v>-0.1485172565297637</v>
       </c>
       <c r="K8" t="n">
         <v>-0.01611086368443455</v>
@@ -1150,35 +1150,35 @@
         <v>-0.0298889126835565</v>
       </c>
       <c r="U8" t="n">
-        <v>0.02113625930995764</v>
+        <v>0.021140415822124</v>
       </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="n">
-        <v>0.009687751875510072</v>
+        <v>0.009687636675505467</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.03766542323461693</v>
+        <v>-0.03765566665822666</v>
       </c>
       <c r="Y8" t="n">
         <v>0.003045803641832145</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.2945444049337761</v>
+        <v>0.2945449216057968</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.01864004800960192</v>
+        <v>0.01863663837746554</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.01864004800960192</v>
+        <v>0.01863663837746554</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.01864004800960192</v>
+        <v>0.01863663837746554</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.01864004800960192</v>
+        <v>0.01863663837746554</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.01864004800960192</v>
+        <v>0.01863663837746554</v>
       </c>
     </row>
     <row r="9">
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.6635507740300308</v>
+        <v>0.6635503125580123</v>
       </c>
       <c r="D9" t="n">
         <v>0.01752971628518865</v>
@@ -1209,10 +1209,10 @@
         <v>0.000364514126580565</v>
       </c>
       <c r="I9" t="n">
-        <v>0.008653350586134024</v>
+        <v>0.008653490362139615</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.01803568918372752</v>
+        <v>-0.01803638806418953</v>
       </c>
       <c r="K9" t="n">
         <v>-0.002746737613869504</v>
@@ -1245,35 +1245,35 @@
         <v>-0.007030070873202833</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.8967884991730629</v>
+        <v>-0.8967865177329837</v>
       </c>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="n">
-        <v>0.009567367390694694</v>
+        <v>0.009566071294642849</v>
       </c>
       <c r="X9" t="n">
-        <v>-0.01620400864816034</v>
+        <v>-0.01619171949566878</v>
       </c>
       <c r="Y9" t="n">
         <v>-0.002616474632658985</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.001943487341739494</v>
+        <v>-0.00194321950172878</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.00960941606437664</v>
+        <v>0.009605437920217516</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.00960941606437664</v>
+        <v>0.009605437920217516</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.00960941606437664</v>
+        <v>0.009605437920217516</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.00960941606437664</v>
+        <v>0.009605437920217516</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.00960941606437664</v>
+        <v>0.009605437920217516</v>
       </c>
     </row>
     <row r="10">
@@ -1288,7 +1288,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0188455650098226</v>
+        <v>0.0188457426098297</v>
       </c>
       <c r="D10" t="n">
         <v>0.003197859583914383</v>
@@ -1304,10 +1304,10 @@
         <v>0.03064438672977546</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.004682444251297769</v>
+        <v>-0.004682604091304162</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.01008600339638462</v>
+        <v>-0.01008622539663594</v>
       </c>
       <c r="K10" t="n">
         <v>0.0219209725568389</v>
@@ -1340,35 +1340,35 @@
         <v>0.01375852624634105</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.001353948198190423</v>
+        <v>-0.001356994086312331</v>
       </c>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="n">
-        <v>0.005849140361965613</v>
+        <v>0.005849864873994594</v>
       </c>
       <c r="X10" t="n">
-        <v>-0.01003553665742146</v>
+        <v>-0.01004700971388039</v>
       </c>
       <c r="Y10" t="n">
         <v>0.004825716577028663</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.00605616053024642</v>
+        <v>-0.006060379058415162</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.0191956674238267</v>
+        <v>0.01920050697602027</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.0191956674238267</v>
+        <v>0.01920050697602027</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.0191956674238267</v>
+        <v>0.01920050697602027</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.0191956674238267</v>
+        <v>0.01920050697602027</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.0191956674238267</v>
+        <v>0.01920050697602027</v>
       </c>
     </row>
     <row r="11">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.01810523813220952</v>
+        <v>0.0181052175882087</v>
       </c>
       <c r="D11" t="n">
         <v>0.007627171025086841</v>
@@ -1399,10 +1399,10 @@
         <v>-0.001071932202877288</v>
       </c>
       <c r="I11" t="n">
-        <v>0.008730098077203921</v>
+        <v>0.008730301501212059</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.005149100326614501</v>
+        <v>-0.005149466854753365</v>
       </c>
       <c r="K11" t="n">
         <v>-0.001421418968856759</v>
@@ -1435,35 +1435,35 @@
         <v>-0.00319211475168459</v>
       </c>
       <c r="U11" t="n">
-        <v>0.006597715944066983</v>
+        <v>0.006598974792117368</v>
       </c>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="n">
-        <v>0.01836895081475803</v>
+        <v>0.01836942659077706</v>
       </c>
       <c r="X11" t="n">
-        <v>0.008870991618839663</v>
+        <v>0.008873154786926192</v>
       </c>
       <c r="Y11" t="n">
         <v>-0.01424320290572811</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.002973840118953605</v>
+        <v>0.002972746102909844</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.00887505078700203</v>
+        <v>-0.008877163171086526</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.00887505078700203</v>
+        <v>-0.008877163171086526</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.00887505078700203</v>
+        <v>-0.008877163171086526</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.00887505078700203</v>
+        <v>-0.008877163171086526</v>
       </c>
       <c r="AE11" t="n">
-        <v>-0.00887505078700203</v>
+        <v>-0.008877163171086526</v>
       </c>
     </row>
     <row r="12">
@@ -1478,7 +1478,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.09969910881996433</v>
+        <v>0.09969899237195967</v>
       </c>
       <c r="D12" t="n">
         <v>-0.004942293317691732</v>
@@ -1494,10 +1494,10 @@
         <v>0.01309334375573375</v>
       </c>
       <c r="I12" t="n">
-        <v>0.003578252207130088</v>
+        <v>0.003578666639146665</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.0286308661853345</v>
+        <v>-0.02863119028203516</v>
       </c>
       <c r="K12" t="n">
         <v>0.01189987065199482</v>
@@ -1530,35 +1530,35 @@
         <v>0.01004867291394692</v>
       </c>
       <c r="U12" t="n">
-        <v>0.09906847918111682</v>
+        <v>0.09906664164504328</v>
       </c>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="n">
-        <v>0.02836627140665085</v>
+        <v>0.0283660825746433</v>
       </c>
       <c r="X12" t="n">
-        <v>-0.01300373351214934</v>
+        <v>-0.01301605972064239</v>
       </c>
       <c r="Y12" t="n">
         <v>0.01067973825118953</v>
       </c>
       <c r="Z12" t="n">
-        <v>-0.01023100533724021</v>
+        <v>-0.01023645813745832</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.01511509356460374</v>
+        <v>0.01512144713285788</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.01511509356460374</v>
+        <v>0.01512144713285788</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.01511509356460374</v>
+        <v>0.01512144713285788</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.01511509356460374</v>
+        <v>0.01512144713285788</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.01511509356460374</v>
+        <v>0.01512144713285788</v>
       </c>
     </row>
     <row r="13">
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.4509245583249822</v>
+        <v>-0.450924427764977</v>
       </c>
       <c r="D13" t="n">
         <v>-0.002908193588327743</v>
@@ -1585,10 +1585,10 @@
         <v>0.01952371537294861</v>
       </c>
       <c r="I13" t="n">
-        <v>0.001066934442677378</v>
+        <v>0.00106683450667338</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.01454006350202984</v>
+        <v>-0.01453981385436839</v>
       </c>
       <c r="K13" t="n">
         <v>0.01660424312816972</v>
@@ -1621,35 +1621,35 @@
         <v>0.01641982203279288</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.07259769621765019</v>
+        <v>-0.07259697295362125</v>
       </c>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="n">
-        <v>-0.009586298111451922</v>
+        <v>-0.009587133503485338</v>
       </c>
       <c r="X13" t="n">
-        <v>0.002490714339628573</v>
+        <v>0.00249734400389376</v>
       </c>
       <c r="Y13" t="n">
         <v>0.01275411679816467</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.008967321382692853</v>
+        <v>0.008969070598762823</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.004114479908579196</v>
+        <v>0.004111346180453846</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.004114479908579196</v>
+        <v>0.004111346180453846</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.004114479908579196</v>
+        <v>0.004111346180453846</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.004114479908579196</v>
+        <v>0.004111346180453846</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.004114479908579196</v>
+        <v>0.004111346180453846</v>
       </c>
     </row>
     <row r="14">
@@ -1664,7 +1664,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.01969963518798541</v>
+        <v>-0.01969953957198158</v>
       </c>
       <c r="D14" t="n">
         <v>-0.03053229702929188</v>
@@ -1680,10 +1680,10 @@
         <v>0.0074490650019626</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.01870829786833191</v>
+        <v>-0.01870844186833767</v>
       </c>
       <c r="J14" t="n">
-        <v>0.005693195997292409</v>
+        <v>0.005693016717421569</v>
       </c>
       <c r="K14" t="n">
         <v>0.002137764661510586</v>
@@ -1716,35 +1716,35 @@
         <v>-0.001856561930262477</v>
       </c>
       <c r="U14" t="n">
-        <v>0.002692344875758411</v>
+        <v>0.002694428747841816</v>
       </c>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="n">
-        <v>-0.0001483543739341749</v>
+        <v>-0.0001477842299113692</v>
       </c>
       <c r="X14" t="n">
-        <v>0.009514508444580336</v>
+        <v>0.00952521177300847</v>
       </c>
       <c r="Y14" t="n">
         <v>-0.003784385335375413</v>
       </c>
       <c r="Z14" t="n">
-        <v>-0.01275607414224296</v>
+        <v>-0.0127555473902219</v>
       </c>
       <c r="AA14" t="n">
-        <v>-0.006237376377495055</v>
+        <v>-0.006240156729606269</v>
       </c>
       <c r="AB14" t="n">
-        <v>-0.006237376377495055</v>
+        <v>-0.006240156729606269</v>
       </c>
       <c r="AC14" t="n">
-        <v>-0.006237376377495055</v>
+        <v>-0.006240156729606269</v>
       </c>
       <c r="AD14" t="n">
-        <v>-0.006237376377495055</v>
+        <v>-0.006240156729606269</v>
       </c>
       <c r="AE14" t="n">
-        <v>-0.006237376377495055</v>
+        <v>-0.006240156729606269</v>
       </c>
     </row>
     <row r="15">
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.00049058325162333</v>
+        <v>0.0004906833796273351</v>
       </c>
       <c r="D15" t="n">
         <v>0.002746113805844552</v>
@@ -1775,10 +1775,10 @@
         <v>0.005684687939387516</v>
       </c>
       <c r="I15" t="n">
-        <v>0.01110231394809256</v>
+        <v>0.0111021851160874</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.007596459100620415</v>
+        <v>-0.007596493036804144</v>
       </c>
       <c r="K15" t="n">
         <v>0.008316471980658879</v>
@@ -1811,35 +1811,35 @@
         <v>0.0100593350583734</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.01049970037224001</v>
+        <v>-0.01050101662829269</v>
       </c>
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="n">
-        <v>0.002615175272607011</v>
+        <v>0.002615112680604507</v>
       </c>
       <c r="X15" t="n">
-        <v>0.001351273590050943</v>
+        <v>0.001349387285975491</v>
       </c>
       <c r="Y15" t="n">
         <v>0.001504612284184491</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.009036895273475809</v>
+        <v>0.009042939913717594</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.004283962827358512</v>
+        <v>0.004285253643410145</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.004283962827358512</v>
+        <v>0.004285253643410145</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.004283962827358512</v>
+        <v>0.004285253643410145</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.004283962827358512</v>
+        <v>0.004285253643410145</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.004283962827358512</v>
+        <v>0.004285253643410145</v>
       </c>
     </row>
     <row r="16">
@@ -1854,7 +1854,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.006747957197918287</v>
+        <v>0.006747253709890147</v>
       </c>
       <c r="D16" t="n">
         <v>-0.004229653321186132</v>
@@ -1870,10 +1870,10 @@
         <v>0.004056001122240045</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.01611475869259034</v>
+        <v>-0.01611449354057974</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.01448138978758432</v>
+        <v>-0.01448108925991935</v>
       </c>
       <c r="K16" t="n">
         <v>0.01865071015402841</v>
@@ -1906,35 +1906,35 @@
         <v>0.02816518327060732</v>
       </c>
       <c r="U16" t="n">
-        <v>0.0030388067296252</v>
+        <v>0.003040815913705616</v>
       </c>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="n">
-        <v>0.01412234869289395</v>
+        <v>0.01412146722085869</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.01141968448878738</v>
+        <v>-0.0114141650645666</v>
       </c>
       <c r="Y16" t="n">
         <v>0.001170574030822961</v>
       </c>
       <c r="Z16" t="n">
-        <v>-0.01501123567244942</v>
+        <v>-0.01500941724037669</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.01062148669685947</v>
+        <v>0.0106198674647947</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.01062148669685947</v>
+        <v>0.0106198674647947</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.01062148669685947</v>
+        <v>0.0106198674647947</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.01062148669685947</v>
+        <v>0.0106198674647947</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.01062148669685947</v>
+        <v>0.0106198674647947</v>
       </c>
     </row>
     <row r="17">
@@ -1949,7 +1949,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.0008313696332547853</v>
+        <v>-0.0008308550732342028</v>
       </c>
       <c r="D17" t="n">
         <v>0.001087392523495701</v>
@@ -1965,10 +1965,10 @@
         <v>0.008068310050732401</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.007696754323870172</v>
+        <v>-0.007696858387874335</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0005061465330961874</v>
+        <v>0.0005060374291037848</v>
       </c>
       <c r="K17" t="n">
         <v>0.001862357834494313</v>
@@ -2001,35 +2001,35 @@
         <v>-0.0009193013167720526</v>
       </c>
       <c r="U17" t="n">
-        <v>0.02851224330117403</v>
+        <v>0.02851107469312726</v>
       </c>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="n">
-        <v>0.01910042466801698</v>
+        <v>0.01909930895597236</v>
       </c>
       <c r="X17" t="n">
-        <v>0.02244623849784954</v>
+        <v>0.02244069488162779</v>
       </c>
       <c r="Y17" t="n">
         <v>0.01156087102243484</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.00894046701361868</v>
+        <v>0.008937542565501701</v>
       </c>
       <c r="AA17" t="n">
-        <v>-0.008991044999641798</v>
+        <v>-0.008987915207516609</v>
       </c>
       <c r="AB17" t="n">
-        <v>-0.008991044999641798</v>
+        <v>-0.008987915207516609</v>
       </c>
       <c r="AC17" t="n">
-        <v>-0.008991044999641798</v>
+        <v>-0.008987915207516609</v>
       </c>
       <c r="AD17" t="n">
-        <v>-0.008991044999641798</v>
+        <v>-0.008987915207516609</v>
       </c>
       <c r="AE17" t="n">
-        <v>-0.008991044999641798</v>
+        <v>-0.008987915207516609</v>
       </c>
     </row>
     <row r="18">
@@ -2040,7 +2040,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.00649382176375287</v>
+        <v>-0.006493129699725188</v>
       </c>
       <c r="D18" t="n">
         <v>1.123824044952962e-05</v>
@@ -2056,10 +2056,10 @@
         <v>0.017880824971233</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.001580172831206913</v>
+        <v>-0.001580266047210642</v>
       </c>
       <c r="J18" t="n">
-        <v>0.002019106500156359</v>
+        <v>0.002019101220204597</v>
       </c>
       <c r="K18" t="n">
         <v>0.009667006754680268</v>
@@ -2092,35 +2092,35 @@
         <v>0.006293785787751431</v>
       </c>
       <c r="U18" t="n">
-        <v>0.0062041400243145</v>
+        <v>0.006200194232156574</v>
       </c>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="n">
-        <v>-0.01218789168751567</v>
+        <v>-0.01218738365549535</v>
       </c>
       <c r="X18" t="n">
-        <v>0.01172047083681883</v>
+        <v>0.01170673784426951</v>
       </c>
       <c r="Y18" t="n">
         <v>0.03970264718810588</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.02346729588269183</v>
+        <v>0.02346812167472486</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.001511091420443657</v>
+        <v>0.001517292924691717</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.001511091420443657</v>
+        <v>0.001517292924691717</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.001511091420443657</v>
+        <v>0.001517292924691717</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.001511091420443657</v>
+        <v>0.001517292924691717</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.001511091420443657</v>
+        <v>0.001517292924691717</v>
       </c>
     </row>
     <row r="19">
@@ -2135,7 +2135,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.003362152550486102</v>
+        <v>0.003362830694513227</v>
       </c>
       <c r="D19" t="n">
         <v>0.005544996989799878</v>
@@ -2151,10 +2151,10 @@
         <v>0.01502727324109093</v>
       </c>
       <c r="I19" t="n">
-        <v>0.01750272050810881</v>
+        <v>0.01750269718010788</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.0159206911115744</v>
+        <v>-0.01592050583194878</v>
       </c>
       <c r="K19" t="n">
         <v>0.01030659977226399</v>
@@ -2187,35 +2187,35 @@
         <v>0.002980425911217036</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.02732836078979031</v>
+        <v>-0.02733088328589128</v>
       </c>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="n">
-        <v>0.006953656502146259</v>
+        <v>0.006952232246089289</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.02206381893055276</v>
+        <v>-0.02207457909098316</v>
       </c>
       <c r="Y19" t="n">
         <v>-0.008198073159922924</v>
       </c>
       <c r="Z19" t="n">
-        <v>-0.009723768676950746</v>
+        <v>-0.009726780101071203</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.01864844608993784</v>
+        <v>0.01865269466610778</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.01864844608993784</v>
+        <v>0.01865269466610778</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.01864844608993784</v>
+        <v>0.01865269466610778</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.01864844608993784</v>
+        <v>0.01865269466610778</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.01864844608993784</v>
+        <v>0.01865269466610778</v>
       </c>
     </row>
     <row r="20">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.01191972614078905</v>
+        <v>-0.01191979353279174</v>
       </c>
       <c r="D20" t="n">
         <v>-0.0007818678072747121</v>
@@ -2246,10 +2246,10 @@
         <v>0.01584765816990633</v>
       </c>
       <c r="I20" t="n">
-        <v>0.005443907545756301</v>
+        <v>0.005443865017754601</v>
       </c>
       <c r="J20" t="n">
-        <v>-8.657457960842846e-05</v>
+        <v>-8.646446760591414e-05</v>
       </c>
       <c r="K20" t="n">
         <v>0.00629648473185939</v>
@@ -2282,35 +2282,35 @@
         <v>-0.0004331198573247943</v>
       </c>
       <c r="U20" t="n">
-        <v>0.01991771508518663</v>
+        <v>0.01991474926106792</v>
       </c>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="n">
-        <v>0.006249415833976632</v>
+        <v>0.006248452473938098</v>
       </c>
       <c r="X20" t="n">
-        <v>0.004932453893298156</v>
+        <v>0.004920834244833369</v>
       </c>
       <c r="Y20" t="n">
         <v>0.01457264717490588</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.003093453723738149</v>
+        <v>0.003098039067921562</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.0009464988858599552</v>
+        <v>0.0009513616700544666</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.0009464988858599552</v>
+        <v>0.0009513616700544666</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.0009464988858599552</v>
+        <v>0.0009513616700544666</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.0009464988858599552</v>
+        <v>0.0009513616700544666</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.0009464988858599552</v>
+        <v>0.0009513616700544666</v>
       </c>
     </row>
     <row r="21">
@@ -2321,7 +2321,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.01869116215564648</v>
+        <v>-0.0186905875956235</v>
       </c>
       <c r="D21" t="n">
         <v>0.002703635724145429</v>
@@ -2337,10 +2337,10 @@
         <v>0.01596776022271041</v>
       </c>
       <c r="I21" t="n">
-        <v>0.01924330521773221</v>
+        <v>0.01924329993773199</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.02266382062462804</v>
+        <v>-0.02266375822516937</v>
       </c>
       <c r="K21" t="n">
         <v>0.01584654159386166</v>
@@ -2373,35 +2373,35 @@
         <v>0.01458498355939934</v>
       </c>
       <c r="U21" t="n">
-        <v>0.01455769603865723</v>
+        <v>0.01455466954253609</v>
       </c>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="n">
-        <v>0.003954263966170558</v>
+        <v>0.003954699806187992</v>
       </c>
       <c r="X21" t="n">
-        <v>-0.01926344141053766</v>
+        <v>-0.01927039977881599</v>
       </c>
       <c r="Y21" t="n">
         <v>0.01036382643055305</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.001422841880913675</v>
+        <v>0.001421155064846203</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.02231851308474052</v>
+        <v>0.02232071426882857</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.02231851308474052</v>
+        <v>0.02232071426882857</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.02231851308474052</v>
+        <v>0.02232071426882857</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.02231851308474052</v>
+        <v>0.02232071426882857</v>
       </c>
       <c r="AE21" t="n">
-        <v>0.02231851308474052</v>
+        <v>0.02232071426882857</v>
       </c>
     </row>
     <row r="22">
@@ -2412,7 +2412,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.02518040347121613</v>
+        <v>-0.02518016299120652</v>
       </c>
       <c r="D22" t="n">
         <v>-0.007685123731404949</v>
@@ -2428,10 +2428,10 @@
         <v>-0.002924413364976535</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.008865450978618038</v>
+        <v>-0.008865614946624597</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.01847073955386042</v>
+        <v>-0.01847069419430183</v>
       </c>
       <c r="K22" t="n">
         <v>-0.01912118994884759</v>
@@ -2464,35 +2464,35 @@
         <v>-0.0304108875524355</v>
       </c>
       <c r="U22" t="n">
-        <v>0.01607826707551656</v>
+        <v>0.01607851705952656</v>
       </c>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="n">
-        <v>0.001594332927773317</v>
+        <v>0.001594459551778382</v>
       </c>
       <c r="X22" t="n">
-        <v>-0.01331001672440067</v>
+        <v>-0.01330438862817554</v>
       </c>
       <c r="Y22" t="n">
         <v>-0.002327976861119074</v>
       </c>
       <c r="Z22" t="n">
-        <v>-0.01405260805010432</v>
+        <v>-0.01405424273816971</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.006867779410711176</v>
+        <v>0.006863182738527308</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.006867779410711176</v>
+        <v>0.006863182738527308</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.006867779410711176</v>
+        <v>0.006863182738527308</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.006867779410711176</v>
+        <v>0.006863182738527308</v>
       </c>
       <c r="AE22" t="n">
-        <v>0.006867779410711176</v>
+        <v>0.006863182738527308</v>
       </c>
     </row>
     <row r="23">
@@ -2503,7 +2503,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.002114730324589213</v>
+        <v>0.002113990740559629</v>
       </c>
       <c r="D23" t="n">
         <v>-0.001372140150885606</v>
@@ -2519,10 +2519,10 @@
         <v>-0.01048538873941555</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.001675557187022287</v>
+        <v>-0.001675460707018428</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.01065253940399784</v>
+        <v>-0.01065226201224193</v>
       </c>
       <c r="K23" t="n">
         <v>-0.009785861959434478</v>
@@ -2555,35 +2555,35 @@
         <v>-0.008151919430076777</v>
       </c>
       <c r="U23" t="n">
-        <v>0.008986755143685887</v>
+        <v>0.008984896391611494</v>
       </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="n">
-        <v>-0.002247560153902406</v>
+        <v>-0.002247559577902383</v>
       </c>
       <c r="X23" t="n">
-        <v>0.002766690830667633</v>
+        <v>0.002759128046365121</v>
       </c>
       <c r="Y23" t="n">
         <v>-0.007362892806515712</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.0008447902417916095</v>
+        <v>0.0008408748816349951</v>
       </c>
       <c r="AA23" t="n">
-        <v>-0.003810408920416356</v>
+        <v>-0.003806292920251716</v>
       </c>
       <c r="AB23" t="n">
-        <v>-0.003810408920416356</v>
+        <v>-0.003806292920251716</v>
       </c>
       <c r="AC23" t="n">
-        <v>-0.003810408920416356</v>
+        <v>-0.003806292920251716</v>
       </c>
       <c r="AD23" t="n">
-        <v>-0.003810408920416356</v>
+        <v>-0.003806292920251716</v>
       </c>
       <c r="AE23" t="n">
-        <v>-0.003810408920416356</v>
+        <v>-0.003806292920251716</v>
       </c>
     </row>
     <row r="24">
@@ -2598,7 +2598,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.01230504865220195</v>
+        <v>-0.01230557137222285</v>
       </c>
       <c r="D24" t="n">
         <v>0.01651558885262355</v>
@@ -2614,10 +2614,10 @@
         <v>0.007708004468320179</v>
       </c>
       <c r="I24" t="n">
-        <v>0.01419436472777459</v>
+        <v>0.01419456555978262</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.002976377548055416</v>
+        <v>-0.002976448684129816</v>
       </c>
       <c r="K24" t="n">
         <v>0.01096631304665252</v>
@@ -2650,35 +2650,35 @@
         <v>0.01248390942735638</v>
       </c>
       <c r="U24" t="n">
-        <v>0.0249315684378611</v>
+        <v>0.02492761870970301</v>
       </c>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="n">
-        <v>0.0068610524984421</v>
+        <v>0.006860226418409054</v>
       </c>
       <c r="X24" t="n">
-        <v>-0.005711292996451718</v>
+        <v>-0.005719843140793725</v>
       </c>
       <c r="Y24" t="n">
         <v>0.01078364145534566</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.002005199696207988</v>
+        <v>0.002006673296266932</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.00762560276902411</v>
+        <v>0.007631384657255385</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.00762560276902411</v>
+        <v>0.007631384657255385</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.00762560276902411</v>
+        <v>0.007631384657255385</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.00762560276902411</v>
+        <v>0.007631384657255385</v>
       </c>
       <c r="AE24" t="n">
-        <v>0.00762560276902411</v>
+        <v>0.007631384657255385</v>
       </c>
     </row>
     <row r="25">
@@ -2689,7 +2689,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.01488349528333981</v>
+        <v>-0.01488410526736421</v>
       </c>
       <c r="D25" t="n">
         <v>-0.02022354388094175</v>
@@ -2705,10 +2705,10 @@
         <v>0.02447870469114818</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.0008306902412276094</v>
+        <v>-0.0008306034572241381</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.002749748130609502</v>
+        <v>-0.002749612194669827</v>
       </c>
       <c r="K25" t="n">
         <v>0.01916914847876594</v>
@@ -2741,35 +2741,35 @@
         <v>0.01403220728128829</v>
       </c>
       <c r="U25" t="n">
-        <v>0.005121348876976867</v>
+        <v>0.005123426605060027</v>
       </c>
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="n">
-        <v>0.01789601610784064</v>
+        <v>0.01789863642794546</v>
       </c>
       <c r="X25" t="n">
-        <v>0.00356232225449289</v>
+        <v>0.003570661390826455</v>
       </c>
       <c r="Y25" t="n">
         <v>0.01503642597745704</v>
       </c>
       <c r="Z25" t="n">
-        <v>-0.009983924751356989</v>
+        <v>-0.00998272705530908</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.008486739987469597</v>
+        <v>0.008483743251349729</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.008486739987469597</v>
+        <v>0.008483743251349729</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.008486739987469597</v>
+        <v>0.008483743251349729</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.008486739987469597</v>
+        <v>0.008483743251349729</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.008486739987469597</v>
+        <v>0.008483743251349729</v>
       </c>
     </row>
     <row r="26">
@@ -2784,7 +2784,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.01295984279039371</v>
+        <v>0.01295989165439567</v>
       </c>
       <c r="D26" t="n">
         <v>-0.01490230658009226</v>
@@ -2800,10 +2800,10 @@
         <v>0.02160733478429339</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.007146379677855186</v>
+        <v>-0.007146287805851511</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.00600208517816691</v>
+        <v>-0.006002013562307972</v>
       </c>
       <c r="K26" t="n">
         <v>0.01546246727449869</v>
@@ -2836,35 +2836,35 @@
         <v>0.01032111622084465</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.02083659606596392</v>
+        <v>-0.02083660336196421</v>
       </c>
       <c r="V26" t="inlineStr"/>
       <c r="W26" t="n">
-        <v>-0.01733622040544881</v>
+        <v>-0.01733478280539131</v>
       </c>
       <c r="X26" t="n">
-        <v>-0.008718574716742988</v>
+        <v>-0.008715260028610399</v>
       </c>
       <c r="Y26" t="n">
         <v>0.01781767319270693</v>
       </c>
       <c r="Z26" t="n">
-        <v>-0.02636911055876442</v>
+        <v>-0.02636701199868047</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.01765647517025901</v>
+        <v>0.01765547120221885</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.01765647517025901</v>
+        <v>0.01765547120221885</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.01765647517025901</v>
+        <v>0.01765547120221885</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.01765647517025901</v>
+        <v>0.01765547120221885</v>
       </c>
       <c r="AE26" t="n">
-        <v>0.01765647517025901</v>
+        <v>0.01765547120221885</v>
       </c>
     </row>
     <row r="27">
@@ -2875,7 +2875,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.005341647477665898</v>
+        <v>0.005341897077675882</v>
       </c>
       <c r="D27" t="n">
         <v>0.01960177316807092</v>
@@ -2891,10 +2891,10 @@
         <v>-0.01450509610020384</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0122383325855333</v>
+        <v>0.01223835360953414</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.00799616942128034</v>
+        <v>-0.007996003389465324</v>
       </c>
       <c r="K27" t="n">
         <v>-0.007011615928464636</v>
@@ -2927,35 +2927,35 @@
         <v>-0.001766803654672146</v>
       </c>
       <c r="U27" t="n">
-        <v>-0.008602549832308456</v>
+        <v>-0.008598738824155922</v>
       </c>
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="n">
-        <v>0.01196371199854848</v>
+        <v>0.01196546390261856</v>
       </c>
       <c r="X27" t="n">
-        <v>-0.001741396293655851</v>
+        <v>-0.001728091077123643</v>
       </c>
       <c r="Y27" t="n">
         <v>-0.01034929020597161</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.005423216376928654</v>
+        <v>0.005421827448873097</v>
       </c>
       <c r="AA27" t="n">
-        <v>-0.00167847625913905</v>
+        <v>-0.001684141891365675</v>
       </c>
       <c r="AB27" t="n">
-        <v>-0.00167847625913905</v>
+        <v>-0.001684141891365675</v>
       </c>
       <c r="AC27" t="n">
-        <v>-0.00167847625913905</v>
+        <v>-0.001684141891365675</v>
       </c>
       <c r="AD27" t="n">
-        <v>-0.00167847625913905</v>
+        <v>-0.001684141891365675</v>
       </c>
       <c r="AE27" t="n">
-        <v>-0.00167847625913905</v>
+        <v>-0.001684141891365675</v>
       </c>
     </row>
     <row r="28">
@@ -2970,7 +2970,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.01360968947238758</v>
+        <v>0.01360985689639427</v>
       </c>
       <c r="D28" t="n">
         <v>0.01176916271076651</v>
@@ -2986,10 +2986,10 @@
         <v>-0.02523759172950367</v>
       </c>
       <c r="I28" t="n">
-        <v>0.01803662971346519</v>
+        <v>0.01803643886545755</v>
       </c>
       <c r="J28" t="n">
-        <v>0.01485666493922579</v>
+        <v>0.01485664953158171</v>
       </c>
       <c r="K28" t="n">
         <v>-0.02413725168549007</v>
@@ -3022,35 +3022,35 @@
         <v>-0.02047028827481153</v>
       </c>
       <c r="U28" t="n">
-        <v>0.003910641228519505</v>
+        <v>0.003908231148423044</v>
       </c>
       <c r="V28" t="inlineStr"/>
       <c r="W28" t="n">
-        <v>0.9915892239515688</v>
+        <v>0.9915893233115728</v>
       </c>
       <c r="X28" t="n">
-        <v>-0.003868384570735382</v>
+        <v>-0.00387794300311772</v>
       </c>
       <c r="Y28" t="n">
         <v>-0.03886077438643097</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.03598996348759854</v>
+        <v>0.0359900550716022</v>
       </c>
       <c r="AA28" t="n">
-        <v>-0.03572355570094222</v>
+        <v>-0.035720350164814</v>
       </c>
       <c r="AB28" t="n">
-        <v>-0.03572355570094222</v>
+        <v>-0.035720350164814</v>
       </c>
       <c r="AC28" t="n">
-        <v>-0.03572355570094222</v>
+        <v>-0.035720350164814</v>
       </c>
       <c r="AD28" t="n">
-        <v>-0.03572355570094222</v>
+        <v>-0.035720350164814</v>
       </c>
       <c r="AE28" t="n">
-        <v>-0.03572355570094222</v>
+        <v>-0.035720350164814</v>
       </c>
     </row>
     <row r="29">
@@ -3065,7 +3065,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.0001122169964886798</v>
+        <v>0.0001117032044681282</v>
       </c>
       <c r="D29" t="n">
         <v>-0.01346903641076145</v>
@@ -3081,10 +3081,10 @@
         <v>-0.01669819343592773</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.02396170358246814</v>
+        <v>-0.02396163215846528</v>
       </c>
       <c r="J29" t="n">
-        <v>0.03251252492312204</v>
+        <v>0.03251211092388507</v>
       </c>
       <c r="K29" t="n">
         <v>-0.01935860189434407</v>
@@ -3117,35 +3117,35 @@
         <v>-0.01845766441830658</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.007093643035915968</v>
+        <v>-0.007093325563903263</v>
       </c>
       <c r="V29" t="inlineStr"/>
       <c r="W29" t="n">
-        <v>0.0212123699364948</v>
+        <v>0.02121349380853975</v>
       </c>
       <c r="X29" t="n">
-        <v>0.0149265626130625</v>
+        <v>0.01493028434121137</v>
       </c>
       <c r="Y29" t="n">
         <v>0.001302889876115595</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.01309699549987982</v>
+        <v>0.01309917517996701</v>
       </c>
       <c r="AA29" t="n">
-        <v>-0.01775084067803362</v>
+        <v>-0.01775108951004358</v>
       </c>
       <c r="AB29" t="n">
-        <v>-0.01775084067803362</v>
+        <v>-0.01775108951004358</v>
       </c>
       <c r="AC29" t="n">
-        <v>-0.01775084067803362</v>
+        <v>-0.01775108951004358</v>
       </c>
       <c r="AD29" t="n">
-        <v>-0.01775084067803362</v>
+        <v>-0.01775108951004358</v>
       </c>
       <c r="AE29" t="n">
-        <v>-0.01775084067803362</v>
+        <v>-0.01775108951004358</v>
       </c>
     </row>
     <row r="30">
@@ -3160,7 +3160,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.01531221574848863</v>
+        <v>-0.01531224109248964</v>
       </c>
       <c r="D30" t="n">
         <v>-0.02053317413332696</v>
@@ -3176,10 +3176,10 @@
         <v>-0.01741705836068233</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.02350465428418617</v>
+        <v>-0.02350489130819565</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.005330710734184023</v>
+        <v>-0.005330815470316328</v>
       </c>
       <c r="K30" t="n">
         <v>-0.006360488126419523</v>
@@ -3212,35 +3212,35 @@
         <v>0.001572404990896199</v>
       </c>
       <c r="U30" t="n">
-        <v>0.02031257394899046</v>
+        <v>0.02031544377310532</v>
       </c>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="n">
-        <v>0.1101099917643996</v>
+        <v>0.1101092817483713</v>
       </c>
       <c r="X30" t="n">
-        <v>-0.0103947549437902</v>
+        <v>-0.01039218598368744</v>
       </c>
       <c r="Y30" t="n">
         <v>-0.02759121633564865</v>
       </c>
       <c r="Z30" t="n">
-        <v>-0.01798677479947099</v>
+        <v>-0.01799195927967837</v>
       </c>
       <c r="AA30" t="n">
-        <v>-0.001758102214324088</v>
+        <v>-0.001760231590409263</v>
       </c>
       <c r="AB30" t="n">
-        <v>-0.001758102214324088</v>
+        <v>-0.001760231590409263</v>
       </c>
       <c r="AC30" t="n">
-        <v>-0.001758102214324088</v>
+        <v>-0.001760231590409263</v>
       </c>
       <c r="AD30" t="n">
-        <v>-0.001758102214324088</v>
+        <v>-0.001760231590409263</v>
       </c>
       <c r="AE30" t="n">
-        <v>-0.001758102214324088</v>
+        <v>-0.001760231590409263</v>
       </c>
     </row>
     <row r="31">
@@ -3255,7 +3255,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.004236238633449544</v>
+        <v>-0.004235327881413114</v>
       </c>
       <c r="D31" t="n">
         <v>-0.002391382367655294</v>
@@ -3271,10 +3271,10 @@
         <v>-0.003690063891602556</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0128929825317193</v>
+        <v>0.01289313353972534</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.009761446630857094</v>
+        <v>-0.009761957687112681</v>
       </c>
       <c r="K31" t="n">
         <v>-0.001140231213609248</v>
@@ -3307,35 +3307,35 @@
         <v>1.480732859229314e-05</v>
       </c>
       <c r="U31" t="n">
-        <v>-0.008842845329926042</v>
+        <v>-0.008843479601951428</v>
       </c>
       <c r="V31" t="inlineStr"/>
       <c r="W31" t="n">
-        <v>0.01074921575796863</v>
+        <v>0.0107483625099345</v>
       </c>
       <c r="X31" t="n">
-        <v>-0.001512119484484779</v>
+        <v>-0.001516654812666192</v>
       </c>
       <c r="Y31" t="n">
         <v>-0.008816976640679064</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.00653469702938788</v>
+        <v>0.006532847493313899</v>
       </c>
       <c r="AA31" t="n">
-        <v>-0.003990864639634585</v>
+        <v>-0.003989163135566525</v>
       </c>
       <c r="AB31" t="n">
-        <v>-0.003990864639634585</v>
+        <v>-0.003989163135566525</v>
       </c>
       <c r="AC31" t="n">
-        <v>-0.003990864639634585</v>
+        <v>-0.003989163135566525</v>
       </c>
       <c r="AD31" t="n">
-        <v>-0.003990864639634585</v>
+        <v>-0.003989163135566525</v>
       </c>
       <c r="AE31" t="n">
-        <v>-0.003990864639634585</v>
+        <v>-0.003989163135566525</v>
       </c>
     </row>
     <row r="32">
@@ -3350,7 +3350,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.1458779634991185</v>
+        <v>0.1458777415471096</v>
       </c>
       <c r="D32" t="n">
         <v>-0.001273986386959456</v>
@@ -3366,10 +3366,10 @@
         <v>0.9869956307758251</v>
       </c>
       <c r="I32" t="n">
-        <v>0.2450002896080115</v>
+        <v>0.2450001199760048</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.6120440128539943</v>
+        <v>-0.6120439214286796</v>
       </c>
       <c r="K32" t="n">
         <v>0.9310201602168062</v>
@@ -3402,35 +3402,35 @@
         <v>0.7885932502637298</v>
       </c>
       <c r="U32" t="n">
-        <v>-0.2314915190412166</v>
+        <v>-0.2314958921293916</v>
       </c>
       <c r="V32" t="inlineStr"/>
       <c r="W32" t="n">
-        <v>-0.0223357975014319</v>
+        <v>-0.02233434175737367</v>
       </c>
       <c r="X32" t="n">
-        <v>-0.6491377776455109</v>
+        <v>-0.6491451654218066</v>
       </c>
       <c r="Y32" t="n">
         <v>0.02857808331912333</v>
       </c>
       <c r="Z32" t="n">
-        <v>-0.5946206976728278</v>
+        <v>-0.5946171744726869</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.8582631079305242</v>
+        <v>0.8582645357385813</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.8582631079305242</v>
+        <v>0.8582645357385813</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.8582631079305242</v>
+        <v>0.8582645357385813</v>
       </c>
       <c r="AD32" t="n">
-        <v>0.8582631079305242</v>
+        <v>0.8582645357385813</v>
       </c>
       <c r="AE32" t="n">
-        <v>0.8582631079305242</v>
+        <v>0.8582645357385813</v>
       </c>
     </row>
     <row r="33">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.01030808383632335</v>
+        <v>-0.01030834073233363</v>
       </c>
       <c r="D33" t="n">
         <v>-0.003106481884259275</v>
@@ -3461,10 +3461,10 @@
         <v>-0.006144108149764326</v>
       </c>
       <c r="I33" t="n">
-        <v>0.002551903302076132</v>
+        <v>0.002551541286061651</v>
       </c>
       <c r="J33" t="n">
-        <v>0.006520415311770909</v>
+        <v>0.006520634767936551</v>
       </c>
       <c r="K33" t="n">
         <v>-0.01031240978849639</v>
@@ -3497,35 +3497,35 @@
         <v>-0.01245967931438717</v>
       </c>
       <c r="U33" t="n">
-        <v>0.003777799543202649</v>
+        <v>0.003780701623318802</v>
       </c>
       <c r="V33" t="inlineStr"/>
       <c r="W33" t="n">
-        <v>0.0097033675241347</v>
+        <v>0.009704693572187742</v>
       </c>
       <c r="X33" t="n">
-        <v>0.01547393437895737</v>
+        <v>0.01548664189946567</v>
       </c>
       <c r="Y33" t="n">
         <v>0.02070782338831293</v>
       </c>
       <c r="Z33" t="n">
-        <v>0.01998656988746279</v>
+        <v>0.01998847951953918</v>
       </c>
       <c r="AA33" t="n">
-        <v>-0.01737070571882823</v>
+        <v>-0.01737458267898331</v>
       </c>
       <c r="AB33" t="n">
-        <v>-0.01737070571882823</v>
+        <v>-0.01737458267898331</v>
       </c>
       <c r="AC33" t="n">
-        <v>-0.01737070571882823</v>
+        <v>-0.01737458267898331</v>
       </c>
       <c r="AD33" t="n">
-        <v>-0.01737070571882823</v>
+        <v>-0.01737458267898331</v>
       </c>
       <c r="AE33" t="n">
-        <v>-0.01737070571882823</v>
+        <v>-0.01737458267898331</v>
       </c>
     </row>
     <row r="34">
@@ -3540,7 +3540,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.0007488887339555493</v>
+        <v>-0.0007493165099726603</v>
       </c>
       <c r="D34" t="n">
         <v>0.002479635075185403</v>
@@ -3556,10 +3556,10 @@
         <v>0.00287552699502108</v>
       </c>
       <c r="I34" t="n">
-        <v>0.01341357404054296</v>
+        <v>0.01341391484055659</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.002657372030759266</v>
+        <v>-0.002657442014825962</v>
       </c>
       <c r="K34" t="n">
         <v>0.006100860628034424</v>
@@ -3592,35 +3592,35 @@
         <v>0.007836628441465135</v>
       </c>
       <c r="U34" t="n">
-        <v>-0.02030846318082593</v>
+        <v>-0.02030841786882412</v>
       </c>
       <c r="V34" t="inlineStr"/>
       <c r="W34" t="n">
-        <v>-0.01313522884540915</v>
+        <v>-0.01313615447744618</v>
       </c>
       <c r="X34" t="n">
-        <v>-0.006674038346961533</v>
+        <v>-0.006669591434783657</v>
       </c>
       <c r="Y34" t="n">
         <v>0.0004204228968169158</v>
       </c>
       <c r="Z34" t="n">
-        <v>0.006583663943346556</v>
+        <v>0.006588527687541106</v>
       </c>
       <c r="AA34" t="n">
-        <v>0.008797088127883525</v>
+        <v>0.008795851071834041</v>
       </c>
       <c r="AB34" t="n">
-        <v>0.008797088127883525</v>
+        <v>0.008795851071834041</v>
       </c>
       <c r="AC34" t="n">
-        <v>0.008797088127883525</v>
+        <v>0.008795851071834041</v>
       </c>
       <c r="AD34" t="n">
-        <v>0.008797088127883525</v>
+        <v>0.008795851071834041</v>
       </c>
       <c r="AE34" t="n">
-        <v>0.008797088127883525</v>
+        <v>0.008795851071834041</v>
       </c>
     </row>
     <row r="35">
@@ -3635,7 +3635,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.01779678647187146</v>
+        <v>-0.01779690464787618</v>
       </c>
       <c r="D35" t="n">
         <v>0.007347835109913403</v>
@@ -3651,10 +3651,10 @@
         <v>-0.02476387635055505</v>
       </c>
       <c r="I35" t="n">
-        <v>-0.00579710327188413</v>
+        <v>-0.005797157703886308</v>
       </c>
       <c r="J35" t="n">
-        <v>0.01297258119669718</v>
+        <v>0.01297268833301299</v>
       </c>
       <c r="K35" t="n">
         <v>0.3084191637607665</v>
@@ -3687,35 +3687,35 @@
         <v>0.5291558900622355</v>
       </c>
       <c r="U35" t="n">
-        <v>0.02339211410424598</v>
+        <v>0.02339383068031468</v>
       </c>
       <c r="V35" t="inlineStr"/>
       <c r="W35" t="n">
-        <v>-0.0006255702010228079</v>
+        <v>-0.0006257170810286831</v>
       </c>
       <c r="X35" t="n">
-        <v>0.02627075855483034</v>
+        <v>0.02627319647492786</v>
       </c>
       <c r="Y35" t="n">
         <v>0.01237830270313211</v>
       </c>
       <c r="Z35" t="n">
-        <v>0.02456251106250044</v>
+        <v>0.02456250645450025</v>
       </c>
       <c r="AA35" t="n">
-        <v>0.0486127600565104</v>
+        <v>0.0486105699124228</v>
       </c>
       <c r="AB35" t="n">
-        <v>0.0486127600565104</v>
+        <v>0.0486105699124228</v>
       </c>
       <c r="AC35" t="n">
-        <v>0.0486127600565104</v>
+        <v>0.0486105699124228</v>
       </c>
       <c r="AD35" t="n">
-        <v>0.0486127600565104</v>
+        <v>0.0486105699124228</v>
       </c>
       <c r="AE35" t="n">
-        <v>0.0486127600565104</v>
+        <v>0.0486105699124228</v>
       </c>
     </row>
     <row r="36">
@@ -3730,7 +3730,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>-0.03190111654004466</v>
+        <v>-0.03190058594802343</v>
       </c>
       <c r="D36" t="n">
         <v>-0.005466936218677448</v>
@@ -3746,10 +3746,10 @@
         <v>0.0153446123897845</v>
       </c>
       <c r="I36" t="n">
-        <v>0.00241962201678488</v>
+        <v>0.002419387872775514</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.00251307125674481</v>
+        <v>-0.002512782488793081</v>
       </c>
       <c r="K36" t="n">
         <v>0.01653834565353382</v>
@@ -3782,35 +3782,35 @@
         <v>0.01836469311858772</v>
       </c>
       <c r="U36" t="n">
-        <v>0.02163467894590639</v>
+        <v>0.02163436800189394</v>
       </c>
       <c r="V36" t="inlineStr"/>
       <c r="W36" t="n">
-        <v>0.01618697863147914</v>
+        <v>0.01618695242347809</v>
       </c>
       <c r="X36" t="n">
-        <v>-0.002194029879761195</v>
+        <v>-0.00219681877587275</v>
       </c>
       <c r="Y36" t="n">
         <v>0.01057870151114806</v>
       </c>
       <c r="Z36" t="n">
-        <v>-0.008582097175283885</v>
+        <v>-0.008581496023259839</v>
       </c>
       <c r="AA36" t="n">
-        <v>0.008164431686577267</v>
+        <v>0.008165884646635384</v>
       </c>
       <c r="AB36" t="n">
-        <v>0.008164431686577267</v>
+        <v>0.008165884646635384</v>
       </c>
       <c r="AC36" t="n">
-        <v>0.008164431686577267</v>
+        <v>0.008165884646635384</v>
       </c>
       <c r="AD36" t="n">
-        <v>0.008164431686577267</v>
+        <v>0.008165884646635384</v>
       </c>
       <c r="AE36" t="n">
-        <v>0.008164431686577267</v>
+        <v>0.008165884646635384</v>
       </c>
     </row>
     <row r="37">
@@ -3825,7 +3825,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.004618597240743889</v>
+        <v>0.004617642328705692</v>
       </c>
       <c r="D37" t="n">
         <v>0.01341683295267332</v>
@@ -3841,10 +3841,10 @@
         <v>0.001163787598551504</v>
       </c>
       <c r="I37" t="n">
-        <v>0.01627775306711012</v>
+        <v>0.01627802100312084</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.007729962706184845</v>
+        <v>-0.007729929682368987</v>
       </c>
       <c r="K37" t="n">
         <v>0.003053531162141246</v>
@@ -3877,35 +3877,35 @@
         <v>0.004041049793641991</v>
       </c>
       <c r="U37" t="n">
-        <v>-0.007844849737982267</v>
+        <v>-0.007846484810047709</v>
       </c>
       <c r="V37" t="inlineStr"/>
       <c r="W37" t="n">
-        <v>-0.001486169915446797</v>
+        <v>-0.001485924731436989</v>
       </c>
       <c r="X37" t="n">
-        <v>0.001624932736997309</v>
+        <v>0.001612723072508923</v>
       </c>
       <c r="Y37" t="n">
         <v>-0.01636385777455431</v>
       </c>
       <c r="Z37" t="n">
-        <v>0.01273560089342403</v>
+        <v>0.01273066879722675</v>
       </c>
       <c r="AA37" t="n">
-        <v>-0.002953785334151413</v>
+        <v>-0.002948565621942624</v>
       </c>
       <c r="AB37" t="n">
-        <v>-0.002953785334151413</v>
+        <v>-0.002948565621942624</v>
       </c>
       <c r="AC37" t="n">
-        <v>-0.002953785334151413</v>
+        <v>-0.002948565621942624</v>
       </c>
       <c r="AD37" t="n">
-        <v>-0.002953785334151413</v>
+        <v>-0.002948565621942624</v>
       </c>
       <c r="AE37" t="n">
-        <v>-0.002953785334151413</v>
+        <v>-0.002948565621942624</v>
       </c>
     </row>
     <row r="38">
@@ -3920,7 +3920,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.01880955790438231</v>
+        <v>0.01880913204836528</v>
       </c>
       <c r="D38" t="n">
         <v>0.02909218925968757</v>
@@ -3936,10 +3936,10 @@
         <v>-0.01529779539591181</v>
       </c>
       <c r="I38" t="n">
-        <v>0.002800700368028014</v>
+        <v>0.002800885552035422</v>
       </c>
       <c r="J38" t="n">
-        <v>0.005237848874313541</v>
+        <v>0.005238059306448025</v>
       </c>
       <c r="K38" t="n">
         <v>-0.009995002863800112</v>
@@ -3972,35 +3972,35 @@
         <v>-0.003382486983299479</v>
       </c>
       <c r="U38" t="n">
-        <v>0.001885493787465003</v>
+        <v>0.001888789659596917</v>
       </c>
       <c r="V38" t="inlineStr"/>
       <c r="W38" t="n">
-        <v>0.00150422799616912</v>
+        <v>0.001504757628190305</v>
       </c>
       <c r="X38" t="n">
-        <v>0.00880821529632861</v>
+        <v>0.008820937504837499</v>
       </c>
       <c r="Y38" t="n">
         <v>-0.008281740811269632</v>
       </c>
       <c r="Z38" t="n">
-        <v>0.003661489586459583</v>
+        <v>0.003661397138455885</v>
       </c>
       <c r="AA38" t="n">
-        <v>-0.008170213574808542</v>
+        <v>-0.008174859782994389</v>
       </c>
       <c r="AB38" t="n">
-        <v>-0.008170213574808542</v>
+        <v>-0.008174859782994389</v>
       </c>
       <c r="AC38" t="n">
-        <v>-0.008170213574808542</v>
+        <v>-0.008174859782994389</v>
       </c>
       <c r="AD38" t="n">
-        <v>-0.008170213574808542</v>
+        <v>-0.008174859782994389</v>
       </c>
       <c r="AE38" t="n">
-        <v>-0.008170213574808542</v>
+        <v>-0.008174859782994389</v>
       </c>
     </row>
     <row r="39">
@@ -4015,7 +4015,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.009366786710671466</v>
+        <v>0.009365770742630827</v>
       </c>
       <c r="D39" t="n">
         <v>0.009771227334849092</v>
@@ -4031,10 +4031,10 @@
         <v>-0.00346554925862197</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.002561875110475004</v>
+        <v>-0.00256205050248202</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.01297067526061774</v>
+        <v>-0.01297069926093004</v>
       </c>
       <c r="K39" t="n">
         <v>0.02588512826740513</v>
@@ -4067,35 +4067,35 @@
         <v>0.03984785352991414</v>
       </c>
       <c r="U39" t="n">
-        <v>-0.002096131379895562</v>
+        <v>-0.002095748723880247</v>
       </c>
       <c r="V39" t="inlineStr"/>
       <c r="W39" t="n">
-        <v>0.006676763691070547</v>
+        <v>0.006678843627153745</v>
       </c>
       <c r="X39" t="n">
-        <v>-0.01815247944609917</v>
+        <v>-0.01815457224618289</v>
       </c>
       <c r="Y39" t="n">
         <v>-0.02661168144846725</v>
       </c>
       <c r="Z39" t="n">
-        <v>-0.005993075471723018</v>
+        <v>-0.005995120079804802</v>
       </c>
       <c r="AA39" t="n">
-        <v>0.02617183535087341</v>
+        <v>0.02617334139893365</v>
       </c>
       <c r="AB39" t="n">
-        <v>0.02617183535087341</v>
+        <v>0.02617334139893365</v>
       </c>
       <c r="AC39" t="n">
-        <v>0.02617183535087341</v>
+        <v>0.02617334139893365</v>
       </c>
       <c r="AD39" t="n">
-        <v>0.02617183535087341</v>
+        <v>0.02617334139893365</v>
       </c>
       <c r="AE39" t="n">
-        <v>0.02617183535087341</v>
+        <v>0.02617334139893365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>